<commit_message>
Initial completion without handling the 1 time security warnings.
</commit_message>
<xml_diff>
--- a/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
+++ b/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
@@ -4,20 +4,62 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="01_Login" sheetId="2" r:id="rId2"/>
+    <sheet name="02_Launch_TCode_va01" sheetId="3" r:id="rId3"/>
+    <sheet name="03_va01_create_sales_document" sheetId="4" r:id="rId4"/>
+    <sheet name="04_va01_order_header" sheetId="5" r:id="rId5"/>
+    <sheet name="05_va01_order_details" sheetId="6" r:id="rId6"/>
+    <sheet name="07_va01_exit" sheetId="7" r:id="rId7"/>
+    <sheet name="99_logout" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+  <si>
+    <t>BrowserName</t>
+  </si>
   <si>
     <t>https://sap-hana.mfdemoportal.com:44300/sap/bc/ui2/flp?sap-client=100&amp;sap-language=EN#Shell-home</t>
+  </si>
+  <si>
+    <t>CHROME</t>
+  </si>
+  <si>
+    <t>OrderQuantity</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>s4h_sd_dem</t>
+  </si>
+  <si>
+    <t>EWMS4-02</t>
+  </si>
+  <si>
+    <t>UnitOfMeasure</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Welcome1</t>
   </si>
   <si>
     <t>URL</t>
@@ -165,12 +207,23 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -190,12 +243,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -494,26 +550,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E1" sqref="E1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="86.47265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.859375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.34375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customFormat="1">
+    <row r="1" customFormat="1">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +602,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -538,4 +615,149 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="1" width="9.41796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.87109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created new action to allow iterating through the order details (multiple line numbers, data driven from the local data sheet for that action).  Also added a new output parameter of the order number created.
</commit_message>
<xml_diff>
--- a/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
+++ b/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="05_va01_order_details" sheetId="6" r:id="rId6"/>
     <sheet name="07_va01_exit" sheetId="7" r:id="rId7"/>
     <sheet name="99_logout" sheetId="8" r:id="rId8"/>
+    <sheet name="06_va01_create_new_order" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -553,7 +554,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:H1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -565,7 +566,7 @@
     <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1">
+    <row r="1" ht="14.95" customFormat="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -630,7 +631,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -649,7 +650,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -668,7 +669,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -679,7 +680,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -691,7 +692,7 @@
     <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1">
+    <row r="1" ht="14.95" customFormat="1">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -737,27 +738,46 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
-  <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>